<commit_message>
adding documents replacing mechanism
</commit_message>
<xml_diff>
--- a/XXX-Szablon_listy.xlsx
+++ b/XXX-Szablon_listy.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Zajecia\Projekty\17-Dir_docs_lister\Dir_docs_lister\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1"/>
   </bookViews>
@@ -47,16 +52,16 @@
     <t>Rewizja:</t>
   </si>
   <si>
-    <t>Lista elementów</t>
-  </si>
-  <si>
     <t>Nazwa zespołu/podzespołu</t>
+  </si>
+  <si>
+    <t>Spis dokumentacji wyrobu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -313,19 +318,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -352,12 +345,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -365,6 +358,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -673,7 +678,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -689,78 +694,77 @@
       <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="8"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="11"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="18" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="17"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A8" s="10"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
+    </row>
+    <row r="9" spans="1:4" ht="27" thickBot="1">
+      <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20"/>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="20"/>
-    </row>
-    <row r="9" spans="1:4" ht="27" thickBot="1">
-      <c r="A9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="D7:D8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C2:D2"/>
@@ -772,6 +776,7 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -786,13 +791,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="61" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" style="4" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>

</xml_diff>